<commit_message>
#First VBS work version
</commit_message>
<xml_diff>
--- a/Resources/Акции_buffer.xlsx
+++ b/Resources/Акции_buffer.xlsx
@@ -448,10 +448,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B48"/>
+      <selection activeCell="A3" sqref="A3:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>266.85</v>
+        <v>263.86</v>
       </c>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>146250</v>
+        <v>146750</v>
       </c>
       <c r="E4" s="3" t="n"/>
       <c r="F4" s="3" t="n"/>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>25432</v>
+        <v>22766</v>
       </c>
       <c r="E5" s="3" t="n"/>
       <c r="F5" s="3" t="n"/>
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>948.3</v>
+        <v>778.1</v>
       </c>
       <c r="E6" s="3" t="n"/>
       <c r="F6" s="3" t="n"/>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>222.87</v>
+        <v>221.88</v>
       </c>
       <c r="E7" s="3" t="n"/>
       <c r="F7" s="3" t="n"/>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>848.8</v>
+        <v>843.4</v>
       </c>
       <c r="E8" s="3" t="n"/>
       <c r="F8" s="3" t="n"/>
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>42.54</v>
+        <v>40.15</v>
       </c>
       <c r="E9" s="3" t="n"/>
       <c r="F9" s="3" t="n"/>
@@ -1480,8 +1480,6 @@
       <c r="E48" s="3" t="n"/>
       <c r="F48" s="3" t="n"/>
     </row>
-    <row r="49"/>
-    <row r="50"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>